<commit_message>
add functionality for re-evaluating the accuracy of points
</commit_message>
<xml_diff>
--- a/Data_for_preliminary_aa.xlsx
+++ b/Data_for_preliminary_aa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instruments" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
   <si>
     <t>point_name</t>
   </si>
@@ -35,12 +35,6 @@
     <t>point_type</t>
   </si>
   <si>
-    <t>mse_x</t>
-  </si>
-  <si>
-    <t>mse_y</t>
-  </si>
-  <si>
     <t>cov_xy</t>
   </si>
   <si>
@@ -141,19 +135,38 @@
   </si>
   <si>
     <t>instrument_inventory_number</t>
+  </si>
+  <si>
+    <t>refined</t>
+  </si>
+  <si>
+    <t>rmse_x</t>
+  </si>
+  <si>
+    <t>rmse_y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -176,8 +189,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -460,11 +477,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.77734375" bestFit="1" customWidth="1"/>
@@ -476,38 +493,38 @@
     <col min="8" max="8" width="14.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
         <v>24</v>
-      </c>
-      <c r="H1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -519,12 +536,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -542,12 +559,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -559,12 +576,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -583,17 +600,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="7" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
@@ -606,21 +623,21 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -629,12 +646,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>15</v>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -642,13 +659,22 @@
       <c r="D3">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>14</v>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>100</v>
@@ -656,13 +682,22 @@
       <c r="D4">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>14</v>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -673,6 +708,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -684,7 +720,7 @@
       <selection activeCell="A7" sqref="A7:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
@@ -693,208 +729,208 @@
     <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
         <v>32</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
         <v>33</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
         <v>34</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
         <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add error ellipse parameters
</commit_message>
<xml_diff>
--- a/Data_for_preliminary_aa.xlsx
+++ b/Data_for_preliminary_aa.xlsx
@@ -35,9 +35,6 @@
     <t>point_type</t>
   </si>
   <si>
-    <t>cov_xy</t>
-  </si>
-  <si>
     <t>MT1</t>
   </si>
   <si>
@@ -144,6 +141,9 @@
   </si>
   <si>
     <t>rmse_y</t>
+  </si>
+  <si>
+    <t>corr_xy</t>
   </si>
 </sst>
 </file>
@@ -477,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -495,36 +495,36 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>22</v>
-      </c>
-      <c r="H1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -538,10 +538,10 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -561,10 +561,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -578,10 +578,10 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -601,7 +601,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -623,21 +623,21 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
         <v>39</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>40</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -648,10 +648,10 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -660,10 +660,10 @@
         <v>100</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -671,10 +671,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>100</v>
@@ -694,10 +694,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -717,13 +717,13 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD12"/>
+      <selection activeCell="A4" sqref="A4:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
     <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
@@ -731,206 +731,206 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" t="s">
-        <v>30</v>
-      </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
         <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
         <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
         <v>6</v>
-      </c>
-      <c r="E11" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>